<commit_message>
Initial commit for report app
</commit_message>
<xml_diff>
--- a/referensi_zona.xlsx
+++ b/referensi_zona.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18350" windowHeight="6730"/>
+    <workbookView windowWidth="18350" windowHeight="7180"/>
   </bookViews>
   <sheets>
     <sheet name="Zona" sheetId="1" r:id="rId1"/>
@@ -115,7 +115,7 @@
     <numFmt numFmtId="178" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="179" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,13 +125,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -601,148 +594,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>

</xml_diff>